<commit_message>
Data format and row selection
</commit_message>
<xml_diff>
--- a/additional material/MODELLO FARC partecipanti_da_importare.xlsx
+++ b/additional material/MODELLO FARC partecipanti_da_importare.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\medlar\Desktop\Python_app\placeholder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\medlar\Desktop\Python_app\additional material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D70B6F9-2563-443B-9D99-78E551F2CD99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A169EE7B-6A81-412B-9AF4-4F5E6EEDFC39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="4440" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30675" yWindow="6780" windowWidth="15375" windowHeight="7965" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="elenco" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="803">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="804">
   <si>
     <t>nome</t>
   </si>
@@ -2435,6 +2435,9 @@
   </si>
   <si>
     <t>RSSMRA85T10A562S</t>
+  </si>
+  <si>
+    <t>CCCFBA85D03L219P</t>
   </si>
 </sst>
 </file>
@@ -2895,7 +2898,7 @@
   <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2992,7 +2995,7 @@
         <v>801</v>
       </c>
       <c r="C3" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
     </row>
   </sheetData>

</xml_diff>